<commit_message>
edit hyperbolic file and add function valEiPult
</commit_message>
<xml_diff>
--- a/hyperbolic.xlsx
+++ b/hyperbolic.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\S2\Studi Independen\lateral pile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729461EF-FFF3-4298-87E3-7C5F600DAA80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE160795-1545-4358-870D-DC2940C07CA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F469CFE8-230F-487D-9DEE-6EA72EBFF68B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>d</t>
   </si>
@@ -71,6 +72,27 @@
   <si>
     <t>Ei</t>
   </si>
+  <si>
+    <t>Et</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>fx</t>
+  </si>
+  <si>
+    <t>y=x^3</t>
+  </si>
+  <si>
+    <t>m=3x^2</t>
+  </si>
 </sst>
 </file>
 
@@ -85,12 +107,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -105,9 +133,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,6 +826,112 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$8:$Q$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.4999999999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9999999999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.4999999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7500000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.2499999999999999E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$T$8:$T$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>47.747530074283915</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.101268044856084</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72.455006015428239</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84.808743986000408</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97.162481956572577</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>109.51621992714475</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>121.86995789771692</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>134.22369586828907</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>146.57743383886123</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-730A-4558-9450-6E0F8BDC3270}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -984,6 +1119,479 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A86C-48B3-9902-84CDDBF38168}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$F$2:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$I$2:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-40.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-13.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>67.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>94.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A86C-48B3-9902-84CDDBF38168}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="513206504"/>
+        <c:axId val="513203224"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="513206504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="513203224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="513203224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="513206504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1064,6 +1672,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1581,6 +2229,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2136,13 +3300,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
@@ -2165,6 +3329,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{510B20D6-C5F3-4DEF-A62D-22AF513CFF44}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2470,10 +3675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B7AFFF-F5B0-401C-B8AA-215AFADF0ACC}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2481,7 +3686,7 @@
     <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2489,7 +3694,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2497,7 +3702,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2506,7 +3711,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2514,7 +3719,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2523,7 +3728,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2542,8 +3747,23 @@
       <c r="O7" t="s">
         <v>7</v>
       </c>
+      <c r="P7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" t="s">
+        <v>7</v>
+      </c>
+      <c r="S7" t="s">
+        <v>13</v>
+      </c>
+      <c r="T7" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2567,205 +3787,321 @@
         <f>N8/((N8/$F$18)+(1/$F$19))</f>
         <v>0</v>
       </c>
+      <c r="P8">
+        <f>$F$19*(1-O8/$F$18)^2</f>
+        <v>12226.968611378501</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" ref="Q8:Q10" si="0">Q9-0.0025</f>
+        <v>2.4999999999999992E-3</v>
+      </c>
+      <c r="R8">
+        <f>Q12/((Q12/F18)+(1/F19))</f>
+        <v>97.162481956572577</v>
+      </c>
+      <c r="S8">
+        <f>F19*(1-R8/F18)^2</f>
+        <v>4941.4951882288651</v>
+      </c>
+      <c r="T8">
+        <f>$S$8*(Q8-$Q$12)+$R$8</f>
+        <v>47.747530074283915</v>
+      </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9">
-        <f t="shared" ref="B9:B16" si="0">A9*$B$5</f>
+        <f t="shared" ref="B9:B16" si="1">A9*$B$5</f>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:C16" si="1">0.5*$B$3*(B9/$B$5)^(1/3)</f>
+        <f t="shared" ref="C9:C16" si="2">0.5*$B$3*(B9/$B$5)^(1/3)</f>
         <v>112.5</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:D16" si="2">B9/C9</f>
+        <f t="shared" ref="D9:D16" si="3">B9/C9</f>
         <v>1.1111111111111112E-4</v>
       </c>
       <c r="N9">
-        <f t="shared" ref="N9:N16" si="3">B9</f>
+        <f t="shared" ref="N9:N16" si="4">B9</f>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="O9">
-        <f t="shared" ref="O9:O16" si="4">N9/((N9/$F$18)+(1/$F$19))</f>
+        <f t="shared" ref="O9:O16" si="5">N9/((N9/$F$18)+(1/$F$19))</f>
         <v>97.162481956572577</v>
       </c>
+      <c r="P9">
+        <f>$F$19*(1-O9/$F$18)^2</f>
+        <v>4941.4951882288651</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>4.9999999999999992E-3</v>
+      </c>
+      <c r="T9">
+        <f t="shared" ref="T9:T16" si="6">$S$8*(Q9-$Q$12)+$R$8</f>
+        <v>60.101268044856084</v>
+      </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="2"/>
+        <v>141.74111811317323</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="3"/>
+        <v>1.7637789466313329E-4</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="5"/>
+        <v>142.43834125373638</v>
+      </c>
+      <c r="P10">
+        <f>$F$19*(1-O10/$F$18)^2</f>
+        <v>2654.9417706344739</v>
+      </c>
+      <c r="Q10">
         <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="1"/>
-        <v>141.74111811317323</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="2"/>
-        <v>1.7637789466313329E-4</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="3"/>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="4"/>
-        <v>142.43834125373638</v>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="6"/>
+        <v>72.455006015428239</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>3</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7500000000000006E-2</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>162.25307665958343</v>
       </c>
       <c r="D11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.3112042478354495E-4</v>
       </c>
       <c r="N11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.7500000000000006E-2</v>
       </c>
       <c r="O11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>168.63133398369132</v>
       </c>
+      <c r="P11">
+        <f>$F$19*(1-O11/$F$18)^2</f>
+        <v>1653.8465757462145</v>
+      </c>
+      <c r="Q11">
+        <f>Q12-0.0025</f>
+        <v>0.01</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="6"/>
+        <v>84.808743986000408</v>
+      </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>4</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>178.58261834642244</v>
       </c>
       <c r="D12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.7998245553219407E-4</v>
       </c>
       <c r="N12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.05</v>
       </c>
       <c r="O12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>185.7060838795052</v>
       </c>
+      <c r="P12">
+        <f>$F$19*(1-O12/$F$18)^2</f>
+        <v>1128.219125638982</v>
+      </c>
+      <c r="Q12" s="2">
+        <f>N9</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="6"/>
+        <v>97.162481956572577</v>
+      </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>5</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.25E-2</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>192.37229400112838</v>
       </c>
       <c r="D13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.2489085980142964E-4</v>
       </c>
       <c r="N13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.25E-2</v>
       </c>
       <c r="O13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>197.71803662459655</v>
       </c>
+      <c r="P13">
+        <f>$F$19*(1-O13/$F$18)^2</f>
+        <v>818.49069477435592</v>
+      </c>
+      <c r="Q13">
+        <f>Q12+0.0025</f>
+        <v>1.5000000000000001E-2</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="6"/>
+        <v>109.51621992714475</v>
+      </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>6</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>204.42606669361572</v>
       </c>
       <c r="D14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.6688080543273633E-4</v>
       </c>
       <c r="N14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="O14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>206.62820320185023</v>
       </c>
+      <c r="P14">
+        <f>$F$19*(1-O14/$F$18)^2</f>
+        <v>620.78022538825678</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" ref="Q14:Q16" si="7">Q13+0.0025</f>
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="6"/>
+        <v>121.86995789771692</v>
+      </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>7</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.7500000000000008E-2</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>215.20475806189376</v>
       </c>
       <c r="D15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.0658952333588581E-4</v>
       </c>
       <c r="N15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.7500000000000008E-2</v>
       </c>
       <c r="O15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>213.50063877553092</v>
       </c>
+      <c r="P15">
+        <f>$F$19*(1-O15/$F$18)^2</f>
+        <v>486.92654857531005</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="7"/>
+        <v>0.02</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="6"/>
+        <v>134.22369586828907</v>
+      </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>8</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>224.99999999999997</v>
       </c>
       <c r="D16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.4444444444444452E-4</v>
       </c>
       <c r="N16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="O16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>218.96264733809241</v>
+      </c>
+      <c r="P16">
+        <f>$F$19*(1-O16/$F$18)^2</f>
+        <v>392.12205783114723</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="7"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="6"/>
+        <v>146.57743383886123</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.35">
@@ -2798,6 +4134,390 @@
       <c r="F19" s="1">
         <f>1/D19</f>
         <v>12226.968611378501</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246E9B84-EA35-4296-87F3-FD89F4F2E52D}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>-5</v>
+      </c>
+      <c r="B2">
+        <f>A2^3</f>
+        <v>-125</v>
+      </c>
+      <c r="C2">
+        <f>3*A2^2</f>
+        <v>75</v>
+      </c>
+      <c r="D2">
+        <f>A2</f>
+        <v>-5</v>
+      </c>
+      <c r="E2">
+        <f>D2^2</f>
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F5" si="0">F3-0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <f>F7^3</f>
+        <v>27</v>
+      </c>
+      <c r="H2">
+        <f>3*F7^2</f>
+        <v>27</v>
+      </c>
+      <c r="I2">
+        <f>$H$2*(F2-$F$7)+$G$2</f>
+        <v>-40.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>-4</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B12" si="1">A3^3</f>
+        <v>-64</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C12" si="2">3*A3^2</f>
+        <v>48</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D12" si="3">A3</f>
+        <v>-4</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E12" si="4">D3^2</f>
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I12" si="5">$H$2*(F3-$F$7)+$G$2</f>
+        <v>-27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <f t="shared" ref="A4:A12" si="6">A3+1</f>
+        <v>-3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="1"/>
+        <v>-27</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="3"/>
+        <v>-3</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="5"/>
+        <v>-13.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="1"/>
+        <v>-8</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <f>F7-0.5</f>
+        <v>2.5</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="5"/>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f>F7+0.5</f>
+        <v>3.5</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="5"/>
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F12" si="7">F8+0.5</f>
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="5"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="7"/>
+        <v>4.5</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="5"/>
+        <v>67.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="7"/>
+        <v>5.5</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="5"/>
+        <v>94.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add module csv for export results
</commit_message>
<xml_diff>
--- a/hyperbolic.xlsx
+++ b/hyperbolic.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\S2\Studi Independen\lateral pile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB9D487-F56A-4460-8AD0-08EC1FF942EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB72122-5592-4D03-ACAC-0464661805C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F469CFE8-230F-487D-9DEE-6EA72EBFF68B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId2"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
   <si>
     <t>d</t>
   </si>
@@ -207,6 +208,9 @@
   <si>
     <t>y+dy</t>
   </si>
+  <si>
+    <t>P</t>
+  </si>
 </sst>
 </file>
 
@@ -215,8 +219,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00000E+00"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
-    <numFmt numFmtId="169" formatCode="0.00000"/>
-    <numFmt numFmtId="173" formatCode="0.0000000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -267,8 +271,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1139,31 +1143,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-5.0000000000000001E-3</c:v>
+                  <c:v>-2.9999999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.5000000000000001E-3</c:v>
+                  <c:v>-2.7499999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>-2.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.2499999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.02</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-9.9999999999999985E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-4.9999999999999984E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.5000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.4999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1175,31 +1179,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-11.416023630933434</c:v>
+                  <c:v>-58.617418536482319</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.8621579552440402</c:v>
+                  <c:v>-54.983351759328968</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6917077204453523</c:v>
+                  <c:v>-51.349284982175625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.2455733961347448</c:v>
+                  <c:v>-47.715218205022275</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.799439071824139</c:v>
+                  <c:v>-44.081151427868932</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27.907170423202928</c:v>
+                  <c:v>-36.813017873562231</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41.014901774581709</c:v>
+                  <c:v>-29.544884319255537</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>54.122633125960498</c:v>
+                  <c:v>-22.27675076494884</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>67.230364477339293</c:v>
+                  <c:v>-15.008617210642146</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1245,7 +1249,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>-0.02</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1300,7 +1304,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-4.4284557999975651E-3</c:v>
+                  <c:v>-4.1343438200230495E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1312,7 +1316,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-16.709483126909603</c:v>
+                  <c:v>-66.837926666735029</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1321,6 +1325,210 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-2D70-4AF7-B246-FDDCD8B8EDA2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AC$6:$AC$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AD$6:$AD$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>167.09481676827025</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-35AE-4440-B7B6-B8FFE65D57E0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AC$11:$AC$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-0.02</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.02</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AD$11:$AD$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-66.8379267073081</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-35AE-4440-B7B6-B8FFE65D57E0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AC$14:$AC$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AD$14:$AD$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-66.8379267073081</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-66.8379267073081</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-35AE-4440-B7B6-B8FFE65D57E0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1525,6 +1733,472 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AC$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AB$21:$AB$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3479E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.1342999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0484000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.132962</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AC$21:$AC$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.418959999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66.83793</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>83.547370000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100.2569</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>108.45959999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>108.45959999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4C62-4877-9DE4-66B6AC93993D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$8:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7500000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.25E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.5000000000000011E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.7500000000000008E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1125</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.13750000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.15000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.16250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.17500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.1875</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$8:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.645654586605616</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64.390176143624913</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70.870559056586615</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>76.34299546673175</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>81.126538329791714</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85.404064834003009</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>89.291309173211218</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>92.866703875161377</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>96.186147000564191</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>99.291046931045514</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>102.21303334680786</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>104.9768762854851</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>107.60237903094688</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>110.10565240787429</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>112.49999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2BCB-43F0-BF69-F7538F26AAB6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="676157864"/>
+        <c:axId val="676157208"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="676157864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="676157208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="676157208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="676157864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:title>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1836,7 +2510,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2309,7 +2983,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2858,6 +3532,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4923,6 +5637,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5507,6 +6737,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>174625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73E4A5E1-C27B-4C3B-B91B-2B82D4A53AD6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5935,10 +7201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B7AFFF-F5B0-401C-B8AA-215AFADF0ACC}">
-  <dimension ref="A1:X51"/>
+  <dimension ref="A1:AD51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5954,7 +7220,7 @@
     <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5962,7 +7228,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5970,7 +7236,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -5978,7 +7244,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -5986,7 +7252,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -5994,8 +7260,23 @@
         <f>2.5*B4*B1</f>
         <v>2.5000000000000001E-2</v>
       </c>
+      <c r="AC5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <f>P8*AC6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -6029,8 +7310,15 @@
       <c r="T7" t="s">
         <v>7</v>
       </c>
+      <c r="AC7">
+        <v>0.05</v>
+      </c>
+      <c r="AD7">
+        <f>AC7*P8</f>
+        <v>167.09481676827025</v>
+      </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0</v>
       </c>
@@ -6060,22 +7348,22 @@
       </c>
       <c r="Q8">
         <f t="shared" ref="Q8:Q10" si="1">Q9-0.0025</f>
-        <v>-5.0000000000000001E-3</v>
+        <v>-2.9999999999999995E-2</v>
       </c>
       <c r="R8">
-        <f>Q12/((Q12/F26)+(1/F27))</f>
-        <v>14.799439071824139</v>
+        <f>(Q12/(ABS(Q12/F26)+(1/F27)))</f>
+        <v>-44.081151427868932</v>
       </c>
       <c r="S8">
-        <f>F27*(1-R8/F26)^2</f>
-        <v>2621.5462702757573</v>
+        <f>F27*(1-ABS(R8/F26))^2</f>
+        <v>1453.6267108613392</v>
       </c>
       <c r="T8">
         <f>$S$8*(Q8-$Q$12)+$R$8</f>
-        <v>-11.416023630933434</v>
+        <v>-58.617418536482319</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A9">
         <f>A8+0.5</f>
         <v>0.5</v>
@@ -6106,14 +7394,14 @@
       </c>
       <c r="Q9">
         <f t="shared" si="1"/>
-        <v>-2.5000000000000001E-3</v>
+        <v>-2.7499999999999997E-2</v>
       </c>
       <c r="T9">
         <f t="shared" ref="T9:T16" si="6">$S$8*(Q9-$Q$12)+$R$8</f>
-        <v>-4.8621579552440402</v>
+        <v>-54.983351759328968</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" ref="A10:A24" si="7">A9+0.5</f>
         <v>1</v>
@@ -6144,14 +7432,20 @@
       </c>
       <c r="Q10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2.4999999999999998E-2</v>
       </c>
       <c r="T10">
         <f t="shared" si="6"/>
-        <v>1.6917077204453523</v>
+        <v>-51.349284982175625</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="7"/>
         <v>1.5</v>
@@ -6182,14 +7476,21 @@
       </c>
       <c r="Q11">
         <f>Q12-0.0025</f>
-        <v>2.5000000000000001E-3</v>
+        <v>-2.2499999999999999E-2</v>
       </c>
       <c r="T11">
         <f t="shared" si="6"/>
-        <v>8.2455733961347448</v>
+        <v>-47.715218205022275</v>
+      </c>
+      <c r="AC11">
+        <f>R21</f>
+        <v>-0.02</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="7"/>
         <v>2</v>
@@ -6219,14 +7520,22 @@
         <v>636.92389706999734</v>
       </c>
       <c r="Q12" s="2">
-        <v>5.0000000000000001E-3</v>
+        <v>-0.02</v>
       </c>
       <c r="T12">
         <f t="shared" si="6"/>
-        <v>14.799439071824139</v>
+        <v>-44.081151427868932</v>
+      </c>
+      <c r="AC12">
+        <f>AC11</f>
+        <v>-0.02</v>
+      </c>
+      <c r="AD12">
+        <f>S21</f>
+        <v>-66.8379267073081</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="7"/>
         <v>2.5</v>
@@ -6257,14 +7566,14 @@
       </c>
       <c r="Q13">
         <f>Q12+0.005</f>
-        <v>0.01</v>
+        <v>-1.4999999999999999E-2</v>
       </c>
       <c r="T13">
         <f t="shared" si="6"/>
-        <v>27.907170423202928</v>
+        <v>-36.813017873562231</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="7"/>
         <v>3</v>
@@ -6295,14 +7604,21 @@
       </c>
       <c r="Q14">
         <f t="shared" ref="Q14:Q16" si="10">Q13+0.005</f>
-        <v>1.4999999999999999E-2</v>
+        <v>-9.9999999999999985E-3</v>
       </c>
       <c r="T14">
         <f t="shared" si="6"/>
-        <v>41.014901774581709</v>
+        <v>-29.544884319255537</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <f>AD12</f>
+        <v>-66.8379267073081</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="7"/>
         <v>3.5</v>
@@ -6333,14 +7649,21 @@
       </c>
       <c r="Q15">
         <f t="shared" si="10"/>
-        <v>0.02</v>
+        <v>-4.9999999999999984E-3</v>
       </c>
       <c r="T15">
         <f t="shared" si="6"/>
-        <v>54.122633125960498</v>
+        <v>-22.27675076494884</v>
+      </c>
+      <c r="AC15">
+        <v>0.2</v>
+      </c>
+      <c r="AD15">
+        <f>AD14</f>
+        <v>-66.8379267073081</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="7"/>
         <v>4</v>
@@ -6371,14 +7694,14 @@
       </c>
       <c r="Q16">
         <f t="shared" si="10"/>
-        <v>2.5000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="T16">
         <f t="shared" si="6"/>
-        <v>67.230364477339293</v>
+        <v>-15.008617210642146</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="7"/>
         <v>4.5</v>
@@ -6408,7 +7731,7 @@
         <v>219.27928032497101</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="7"/>
         <v>5</v>
@@ -6438,7 +7761,7 @@
         <v>187.07762801074779</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="7"/>
         <v>5.5</v>
@@ -6468,7 +7791,7 @@
         <v>161.48153947773139</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="7"/>
         <v>6</v>
@@ -6518,8 +7841,17 @@
       <c r="X20" t="s">
         <v>56</v>
       </c>
+      <c r="AA20" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="7"/>
         <v>6.5</v>
@@ -6549,35 +7881,44 @@
         <v>123.85225537468222</v>
       </c>
       <c r="R21">
-        <f>-Q12</f>
-        <v>-5.0000000000000001E-3</v>
+        <f>Q12</f>
+        <v>-0.02</v>
       </c>
       <c r="S21">
-        <f>R21*$P$8</f>
-        <v>-16.709481676827025</v>
+        <f>IF(R21&lt;0,MAX(R21*$P$8,-$F$26),MIN(R21*$P$8,$F$26))</f>
+        <v>-66.8379267073081</v>
       </c>
       <c r="T21">
-        <f>R21/((R21/$F$26)+(1/$F$27))</f>
-        <v>-19.185611726236989</v>
+        <f>(R21)/((ABS(R21)/$F$26)+(1/$F$27))</f>
+        <v>-44.081151427868932</v>
       </c>
       <c r="U21">
         <f>S21-T21</f>
-        <v>2.4761300494099636</v>
+        <v>-22.756775279439168</v>
       </c>
       <c r="V21">
-        <f>$F$27*(1-T21/$F$26)^2</f>
-        <v>4405.7344737436342</v>
+        <f>$F$27*(1-ABS(T21/$F$26))^2</f>
+        <v>1453.6267108613392</v>
       </c>
       <c r="W21">
-        <f>(S21-T21)/$V$21</f>
-        <v>5.6202434898577761E-4</v>
+        <f>(S21-T21)/V21</f>
+        <v>-1.5655171378871232E-2</v>
       </c>
       <c r="X21">
         <f>R21+W21</f>
-        <v>-4.4379756510142228E-3</v>
+        <v>-3.5655171378871232E-2</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+      <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="7"/>
         <v>7</v>
@@ -6608,34 +7949,43 @@
       </c>
       <c r="R22">
         <f>X21</f>
-        <v>-4.4379756510142228E-3</v>
+        <v>-3.5655171378871232E-2</v>
       </c>
       <c r="S22">
         <f>S21</f>
-        <v>-16.709481676827025</v>
+        <v>-66.8379267073081</v>
       </c>
       <c r="T22">
-        <f>R22/((R22/$F$26)+(1/$F$27))</f>
-        <v>-16.750050705894992</v>
+        <f t="shared" ref="T22:T49" si="15">(R22)/((ABS(R22)/$F$26)+(1/$F$27))</f>
+        <v>-62.049230975258659</v>
       </c>
       <c r="U22">
         <f>S22-T22</f>
-        <v>4.0569029067967222E-2</v>
+        <v>-4.7886957320494403</v>
       </c>
       <c r="V22">
-        <f t="shared" ref="V22:V25" si="15">$F$27*(1-T22/$F$26)^2</f>
-        <v>4262.5496216361062</v>
+        <f t="shared" ref="V22:V49" si="16">$F$27*(1-ABS(T22/$F$26))^2</f>
+        <v>906.22236490610237</v>
       </c>
       <c r="W22">
-        <f t="shared" ref="W22:W25" si="16">(S22-T22)/$V$21</f>
-        <v>9.2082328859675843E-6</v>
+        <f t="shared" ref="W22:W49" si="17">(S22-T22)/V22</f>
+        <v>-5.2842391862019623E-3</v>
       </c>
       <c r="X22">
         <f>R22+W22</f>
-        <v>-4.4287674181282552E-3</v>
+        <v>-4.0939410565073192E-2</v>
+      </c>
+      <c r="AA22">
+        <v>0.01</v>
+      </c>
+      <c r="AB22">
+        <v>1.3479E-2</v>
+      </c>
+      <c r="AC22">
+        <v>33.418959999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="7"/>
         <v>7.5</v>
@@ -6666,34 +8016,43 @@
       </c>
       <c r="R23">
         <f>X22</f>
-        <v>-4.4287674181282552E-3</v>
+        <v>-4.0939410565073192E-2</v>
       </c>
       <c r="S23">
-        <f t="shared" ref="S23:S25" si="17">S22</f>
-        <v>-16.709481676827025</v>
+        <f t="shared" ref="S23:S49" si="18">S22</f>
+        <v>-66.8379267073081</v>
       </c>
       <c r="T23">
-        <f t="shared" ref="T23:T25" si="18">R23/((R23/$F$26)+(1/$F$27))</f>
-        <v>-16.710810689761971</v>
+        <f t="shared" si="15"/>
+        <v>-66.520350851216108</v>
       </c>
       <c r="U23">
         <f t="shared" ref="U23:U25" si="19">S23-T23</f>
-        <v>1.3290129349456947E-3</v>
+        <v>-0.31757585609199168</v>
       </c>
       <c r="V23">
-        <f t="shared" si="15"/>
-        <v>4260.2620909618199</v>
+        <f t="shared" si="16"/>
+        <v>790.01059771516293</v>
       </c>
       <c r="W23">
-        <f t="shared" si="16"/>
-        <v>3.0165525018951218E-7</v>
+        <f t="shared" si="17"/>
+        <v>-4.0198936192814615E-4</v>
       </c>
       <c r="X23">
         <f>R23+W23</f>
-        <v>-4.4284657628780658E-3</v>
+        <v>-4.1341399927001338E-2</v>
+      </c>
+      <c r="AA23">
+        <v>0.02</v>
+      </c>
+      <c r="AB23">
+        <v>4.1342999999999998E-2</v>
+      </c>
+      <c r="AC23">
+        <v>66.83793</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="7"/>
         <v>8</v>
@@ -6724,64 +8083,82 @@
       </c>
       <c r="R24">
         <f>X23</f>
-        <v>-4.4284657628780658E-3</v>
+        <v>-4.1341399927001338E-2</v>
       </c>
       <c r="S24">
-        <f t="shared" si="17"/>
-        <v>-16.709481676827025</v>
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
       </c>
       <c r="T24">
-        <f t="shared" si="18"/>
-        <v>-16.709525570633105</v>
+        <f t="shared" si="15"/>
+        <v>-66.836332575265274</v>
       </c>
       <c r="U24">
         <f t="shared" si="19"/>
-        <v>4.3893806079609021E-5</v>
+        <v>-1.5941320428254357E-3</v>
       </c>
       <c r="V24">
-        <f t="shared" si="15"/>
-        <v>4260.1871842140445</v>
+        <f t="shared" si="16"/>
+        <v>782.09928876097092</v>
       </c>
       <c r="W24">
-        <f t="shared" si="16"/>
-        <v>9.962880500674304E-9</v>
+        <f t="shared" si="17"/>
+        <v>-2.038273229158558E-6</v>
       </c>
       <c r="X24">
         <f>R24+W24</f>
-        <v>-4.4284557999975651E-3</v>
+        <v>-4.1343438200230495E-2</v>
+      </c>
+      <c r="AA24">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AB24">
+        <v>7.0484000000000005E-2</v>
+      </c>
+      <c r="AC24">
+        <v>83.547370000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
       <c r="R25">
         <f>X24</f>
-        <v>-4.4284557999975651E-3</v>
+        <v>-4.1343438200230495E-2</v>
       </c>
       <c r="S25">
-        <f t="shared" si="17"/>
-        <v>-16.709481676827025</v>
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
       </c>
       <c r="T25">
-        <f t="shared" si="18"/>
-        <v>-16.709483126909603</v>
+        <f t="shared" si="15"/>
+        <v>-66.837926666735029</v>
       </c>
       <c r="U25">
         <f t="shared" si="19"/>
-        <v>1.4500825784580229E-6</v>
+        <v>-4.0573070236860076E-8</v>
       </c>
       <c r="V25">
-        <f t="shared" si="15"/>
-        <v>4260.1847102746387</v>
+        <f t="shared" si="16"/>
+        <v>782.05947804754953</v>
       </c>
       <c r="W25">
-        <f t="shared" si="16"/>
-        <v>3.2913526384758744E-10</v>
+        <f t="shared" si="17"/>
+        <v>-5.1879775612658984E-11</v>
       </c>
       <c r="X25">
         <f>R25+W25</f>
-        <v>-4.428455470862301E-3</v>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="AA25">
+        <v>0.03</v>
+      </c>
+      <c r="AB25">
+        <v>0.132962</v>
+      </c>
+      <c r="AC25">
+        <v>100.2569</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>9</v>
       </c>
@@ -6796,8 +8173,45 @@
         <f>1/D26</f>
         <v>129.46881674274996</v>
       </c>
+      <c r="R26">
+        <f t="shared" ref="R26:R32" si="20">X25</f>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U26">
+        <f t="shared" ref="U26:U32" si="21">S26-T26</f>
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <f t="shared" ref="X26:X32" si="22">R26+W26</f>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="AA26">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AB26">
+        <v>0.2</v>
+      </c>
+      <c r="AC26">
+        <v>108.45959999999999</v>
+      </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.35">
       <c r="C27" t="s">
         <v>10</v>
       </c>
@@ -6812,35 +8226,334 @@
         <f>1/D27</f>
         <v>3341.8963353654049</v>
       </c>
+      <c r="R27">
+        <f t="shared" si="20"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <f t="shared" si="22"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="AA27">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="AB27">
+        <v>0.2</v>
+      </c>
+      <c r="AC27">
+        <v>108.45959999999999</v>
+      </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="R28">
+        <f t="shared" si="20"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X28">
+        <f t="shared" si="22"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="R29">
+        <f t="shared" si="20"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X29">
+        <f t="shared" si="22"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="R30">
+        <f t="shared" si="20"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="22"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="R31">
+        <f t="shared" si="20"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="22"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="R32">
+        <f t="shared" si="20"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="22"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B33" s="3"/>
+      <c r="R33">
+        <f t="shared" ref="R33:R43" si="23">X32</f>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U33">
+        <f t="shared" ref="U33:U43" si="24">S33-T33</f>
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X33">
+        <f t="shared" ref="X33:X43" si="25">R33+W33</f>
+        <v>-4.1343438252110273E-2</v>
+      </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>20</v>
       </c>
       <c r="B34">
         <v>0.12</v>
       </c>
+      <c r="R34">
+        <f t="shared" si="23"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="25"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>21</v>
       </c>
       <c r="B35" s="3">
         <v>20000000</v>
       </c>
+      <c r="R35">
+        <f t="shared" si="23"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="25"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>0</v>
       </c>
       <c r="B36">
         <v>0.5</v>
       </c>
+      <c r="R36">
+        <f t="shared" si="23"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X36">
+        <f t="shared" si="25"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -6848,8 +8561,36 @@
         <f>(1/64)*PI()*(B36^4)</f>
         <v>3.0679615757712823E-3</v>
       </c>
+      <c r="R37">
+        <f t="shared" si="23"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X37">
+        <f t="shared" si="25"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -6890,8 +8631,36 @@
       <c r="O38" t="s">
         <v>46</v>
       </c>
+      <c r="R38">
+        <f t="shared" si="23"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X38">
+        <f t="shared" si="25"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="K39" s="8">
         <v>1.8499999999999999E-2</v>
       </c>
@@ -6911,8 +8680,36 @@
         <f>K39-N39</f>
         <v>2.733428187230157E-2</v>
       </c>
+      <c r="R39">
+        <f t="shared" si="23"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="V39">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X39">
+        <f t="shared" si="25"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>24</v>
       </c>
@@ -6936,23 +8733,51 @@
         <v>-8.8342818723015706E-3</v>
       </c>
       <c r="L40" s="7">
-        <f t="shared" ref="L40:L45" si="20">K40/((K40/$F$26)+(1/$F$27))</f>
+        <f t="shared" ref="L40:L45" si="26">K40/((K40/$F$26)+(1/$F$27))</f>
         <v>-38.244227086000606</v>
       </c>
       <c r="M40" s="1">
-        <f t="shared" ref="M40:M45" si="21">$F$27*(1-(L40/$F$26))^2</f>
+        <f t="shared" ref="M40:M45" si="27">$F$27*(1-(L40/$F$26))^2</f>
         <v>5607.8488367763657</v>
       </c>
       <c r="N40" s="3">
-        <f t="shared" ref="N40:N45" si="22">K40-(L40/M40)</f>
+        <f t="shared" ref="N40:N45" si="28">K40-(L40/M40)</f>
         <v>-2.0145140434695364E-3</v>
       </c>
       <c r="O40" s="3">
-        <f t="shared" ref="O40:O45" si="23">K40-N40</f>
+        <f t="shared" ref="O40" si="29">K40-N40</f>
         <v>-6.8197678288320343E-3</v>
       </c>
+      <c r="R40">
+        <f t="shared" si="23"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="V40">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X40">
+        <f t="shared" si="25"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -6972,27 +8797,55 @@
         <v>3.1099618532975404</v>
       </c>
       <c r="K41" s="8">
-        <f t="shared" ref="K41:K45" si="24">N40</f>
+        <f t="shared" ref="K41:K45" si="30">N40</f>
         <v>-2.0145140434695364E-3</v>
       </c>
       <c r="L41" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>-7.1015745106225614</v>
       </c>
       <c r="M41" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>3718.5679647373158</v>
       </c>
       <c r="N41" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>-1.0475346413742637E-4</v>
       </c>
       <c r="O41" s="3">
-        <f t="shared" ref="O41:O45" si="25">K41-N41</f>
+        <f t="shared" ref="O41:O45" si="31">K41-N41</f>
         <v>-1.90976057933211E-3</v>
       </c>
+      <c r="R41">
+        <f t="shared" si="23"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U41">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="V41">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X41">
+        <f t="shared" si="25"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -7019,27 +8872,55 @@
         <v>2.6063217636194898E-4</v>
       </c>
       <c r="K42" s="8">
+        <f t="shared" si="30"/>
+        <v>-1.0475346413742637E-4</v>
+      </c>
+      <c r="L42" s="7">
+        <f t="shared" si="26"/>
+        <v>-0.35102436485603283</v>
+      </c>
+      <c r="M42" s="1">
+        <f t="shared" si="27"/>
+        <v>3360.0424394764582</v>
+      </c>
+      <c r="N42" s="3">
+        <f t="shared" si="28"/>
+        <v>-2.832465199586185E-7</v>
+      </c>
+      <c r="O42" s="3">
+        <f t="shared" si="31"/>
+        <v>-1.0447021761746775E-4</v>
+      </c>
+      <c r="R42">
+        <f t="shared" si="23"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U42">
         <f t="shared" si="24"/>
-        <v>-1.0475346413742637E-4</v>
-      </c>
-      <c r="L42" s="7">
-        <f t="shared" si="20"/>
-        <v>-0.35102436485603283</v>
-      </c>
-      <c r="M42" s="1">
-        <f t="shared" si="21"/>
-        <v>3360.0424394764582</v>
-      </c>
-      <c r="N42" s="3">
-        <f t="shared" si="22"/>
-        <v>-2.832465199586185E-7</v>
-      </c>
-      <c r="O42" s="3">
+        <v>0</v>
+      </c>
+      <c r="V42">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X42">
         <f t="shared" si="25"/>
-        <v>-1.0447021761746775E-4</v>
+        <v>-4.1343438252110273E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>27</v>
       </c>
@@ -7055,31 +8936,59 @@
         <v>1.5907434767475822E-6</v>
       </c>
       <c r="I43" s="1">
-        <f t="shared" ref="I43:I44" si="26">H43*100</f>
+        <f t="shared" ref="I43:I44" si="32">H43*100</f>
         <v>1.5907434767475822E-4</v>
       </c>
       <c r="K43" s="8">
+        <f t="shared" si="30"/>
+        <v>-2.832465199586185E-7</v>
+      </c>
+      <c r="L43" s="7">
+        <f t="shared" si="26"/>
+        <v>-9.4658742780389185E-4</v>
+      </c>
+      <c r="M43" s="1">
+        <f t="shared" si="27"/>
+        <v>3341.9452028641581</v>
+      </c>
+      <c r="N43" s="3">
+        <f t="shared" si="28"/>
+        <v>-2.0708896645834402E-12</v>
+      </c>
+      <c r="O43" s="3">
+        <f t="shared" si="31"/>
+        <v>-2.8324444906895391E-7</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="23"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U43">
         <f t="shared" si="24"/>
-        <v>-2.832465199586185E-7</v>
-      </c>
-      <c r="L43" s="7">
-        <f t="shared" si="20"/>
-        <v>-9.4658742780389185E-4</v>
-      </c>
-      <c r="M43" s="1">
-        <f t="shared" si="21"/>
-        <v>3341.9452028641581</v>
-      </c>
-      <c r="N43" s="3">
-        <f t="shared" si="22"/>
-        <v>-2.0708896645834402E-12</v>
-      </c>
-      <c r="O43" s="3">
+        <v>0</v>
+      </c>
+      <c r="V43">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W43">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X43">
         <f t="shared" si="25"/>
-        <v>-2.8324444906895391E-7</v>
+        <v>-4.1343438252110273E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -7102,31 +9011,59 @@
         <v>-5.0571305533594541E-6</v>
       </c>
       <c r="I44" s="1">
+        <f t="shared" si="32"/>
+        <v>-5.0571305533594544E-4</v>
+      </c>
+      <c r="K44" s="8">
+        <f t="shared" si="30"/>
+        <v>-2.0708896645834402E-12</v>
+      </c>
+      <c r="L44" s="7">
         <f t="shared" si="26"/>
-        <v>-5.0571305533594544E-4</v>
-      </c>
-      <c r="K44" s="8">
-        <f t="shared" si="24"/>
-        <v>-2.0708896645834402E-12</v>
-      </c>
-      <c r="L44" s="7">
-        <f t="shared" si="20"/>
         <v>-6.9206985813874348E-9</v>
       </c>
       <c r="M44" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>3341.8963357226839</v>
       </c>
       <c r="N44" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>-1.1069841482718926E-22</v>
       </c>
       <c r="O44" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>-2.0708896644727418E-12</v>
       </c>
+      <c r="R44">
+        <f t="shared" ref="R44:R49" si="33">X43</f>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U44">
+        <f t="shared" ref="U44:U49" si="34">S44-T44</f>
+        <v>0</v>
+      </c>
+      <c r="V44">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W44">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X44">
+        <f t="shared" ref="X44:X49" si="35">R44+W44</f>
+        <v>-4.1343438252110273E-2</v>
+      </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -7139,27 +9076,55 @@
         <v>5.6324043092540437E-6</v>
       </c>
       <c r="K45" s="8">
-        <f t="shared" si="24"/>
+        <f t="shared" si="30"/>
         <v>-1.1069841482718926E-22</v>
       </c>
       <c r="L45" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>-3.6994262684174321E-19</v>
       </c>
       <c r="M45" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="27"/>
         <v>3341.8963353654049</v>
       </c>
       <c r="N45" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="O45" s="3">
-        <f t="shared" si="25"/>
+        <f t="shared" si="31"/>
         <v>-1.1069841482718926E-22</v>
       </c>
+      <c r="R45">
+        <f t="shared" si="33"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T45">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U45">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="V45">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W45">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X45">
+        <f t="shared" si="35"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>30</v>
       </c>
@@ -7167,8 +9132,36 @@
         <f>1/(6+E38-B42-B45*(4-B43))</f>
         <v>0.99975163102820463</v>
       </c>
+      <c r="R46">
+        <f t="shared" si="33"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T46">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U46">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="V46">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W46">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X46">
+        <f t="shared" si="35"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -7176,8 +9169,36 @@
         <f>B46*(4-B45)</f>
         <v>1.9996613134389298</v>
       </c>
+      <c r="R47">
+        <f t="shared" si="33"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T47">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U47">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="V47">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W47">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X47">
+        <f t="shared" si="35"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>32</v>
       </c>
@@ -7185,8 +9206,36 @@
         <f>1/(6+F38-B44-B47*(4-B45))</f>
         <v>0.43909435779642814</v>
       </c>
+      <c r="R48">
+        <f t="shared" si="33"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S48">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T48">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U48">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="V48">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W48">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X48">
+        <f t="shared" si="35"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>33</v>
       </c>
@@ -7194,8 +9243,36 @@
         <f>B48*(4-B47)</f>
         <v>0.87833743095088379</v>
       </c>
+      <c r="R49">
+        <f t="shared" si="33"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="18"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="T49">
+        <f t="shared" si="15"/>
+        <v>-66.8379267073081</v>
+      </c>
+      <c r="U49">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="V49">
+        <f t="shared" si="16"/>
+        <v>782.05947703429354</v>
+      </c>
+      <c r="W49">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="X49">
+        <f t="shared" si="35"/>
+        <v>-4.1343438252110273E-2</v>
+      </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>34</v>
       </c>
@@ -7204,7 +9281,7 @@
         <v>0.26003682408976653</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>35</v>
       </c>
@@ -7220,6 +9297,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63474B9A-71BF-4199-982C-948E3E0E858C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584A5ED7-2322-4994-8EEB-4A9C21CE5D77}">
   <dimension ref="A2"/>
   <sheetViews>
@@ -7240,7 +9331,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F53E62-D71D-47F3-9CE7-DD6F7D6FDC78}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -7353,7 +9444,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246E9B84-EA35-4296-87F3-FD89F4F2E52D}">
   <dimension ref="A1:I12"/>
   <sheetViews>
@@ -7737,7 +9828,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A125BCA6-1EF8-4A09-9A37-7EFAD9FA5477}">
   <dimension ref="A1:P25"/>
   <sheetViews>

</xml_diff>